<commit_message>
Commented out one print
</commit_message>
<xml_diff>
--- a/Analuusitud seletused/Sarnasuse_meetod.xlsx
+++ b/Analuusitud seletused/Sarnasuse_meetod.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\OneDrive\Töölaud\Bakatöö\Lõpptulemus\Protsent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d36e1e23a845f0f8/Töölaud/Seletuste-automaatne-genereerimine-ja-kontrollimine-Eesti-Wordneti-naitel/Analuusitud seletused/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35789C31-F028-4BE1-95E5-0F78BC3008D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{35789C31-F028-4BE1-95E5-0F78BC3008D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7B02BEB-3486-4DB7-B21C-89427D1798CB}"/>
   <bookViews>
-    <workbookView xWindow="6945" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31560" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="526">
   <si>
     <t>Sünohulk</t>
   </si>
@@ -1609,6 +1609,9 @@
   </si>
   <si>
     <t>EKI seletuse hinne</t>
+  </si>
+  <si>
+    <t>Keskmine</t>
   </si>
 </sst>
 </file>
@@ -3148,7 +3151,7 @@
   <dimension ref="A1:M256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3383,6 +3386,9 @@
       <c r="F8" s="11">
         <v>4</v>
       </c>
+      <c r="I8" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -3403,6 +3409,10 @@
       <c r="F9" s="11">
         <v>4</v>
       </c>
+      <c r="I9" s="4">
+        <f>AVERAGE(F2:F256)</f>
+        <v>3.8078431372549018</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -3544,7 +3554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4614</v>
       </c>
@@ -3564,7 +3574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9566</v>
       </c>
@@ -3584,7 +3594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>7518</v>
       </c>
@@ -3604,7 +3614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3041</v>
       </c>
@@ -3624,7 +3634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>6808</v>
       </c>
@@ -3644,7 +3654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>12759</v>
       </c>
@@ -3664,7 +3674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>15481</v>
       </c>
@@ -3684,7 +3694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4686</v>
       </c>
@@ -3704,7 +3714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>9240</v>
       </c>
@@ -3723,12 +3733,8 @@
       <c r="F25" s="11">
         <v>4</v>
       </c>
-      <c r="I25" s="4">
-        <f>AVERAGE(F2:F256)</f>
-        <v>3.8078431372549018</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>13400</v>
       </c>
@@ -3748,7 +3754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>9195</v>
       </c>
@@ -3768,7 +3774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>5911</v>
       </c>
@@ -3788,7 +3794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1234</v>
       </c>
@@ -3808,7 +3814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>10439</v>
       </c>
@@ -3828,7 +3834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>3228</v>
       </c>
@@ -3848,7 +3854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2763</v>
       </c>

</xml_diff>